<commit_message>
updated 9 month size with SN experiment
</commit_message>
<xml_diff>
--- a/Data/Larval-DNA/DNA-extraction-data.xlsx
+++ b/Data/Larval-DNA/DNA-extraction-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28331"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25520" windowHeight="15280" tabRatio="1000" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25520" windowHeight="15280" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="DNA Samples" sheetId="1" r:id="rId1"/>
@@ -3141,8 +3141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C27" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12859,7 +12859,7 @@
   </sheetPr>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -12961,7 +12961,7 @@
         <v>84</v>
       </c>
       <c r="L2" s="138">
-        <f>K2*46</f>
+        <f t="shared" ref="L2:L13" si="0">K2*46</f>
         <v>3864</v>
       </c>
       <c r="M2" s="134"/>
@@ -13003,7 +13003,7 @@
         <v>43.9</v>
       </c>
       <c r="L3" s="138">
-        <f>K3*46</f>
+        <f t="shared" si="0"/>
         <v>2019.3999999999999</v>
       </c>
       <c r="M3" s="134"/>
@@ -13045,7 +13045,7 @@
         <v>56</v>
       </c>
       <c r="L4" s="138">
-        <f>K4*46</f>
+        <f t="shared" si="0"/>
         <v>2576</v>
       </c>
       <c r="M4" s="134"/>
@@ -13087,7 +13087,7 @@
         <v>24.2</v>
       </c>
       <c r="L5" s="138">
-        <f>K5*46</f>
+        <f t="shared" si="0"/>
         <v>1113.2</v>
       </c>
       <c r="M5" s="134"/>
@@ -13129,7 +13129,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="L6" s="138">
-        <f>K6*46</f>
+        <f t="shared" si="0"/>
         <v>1527.2</v>
       </c>
       <c r="M6" s="134"/>
@@ -13171,7 +13171,7 @@
         <v>76</v>
       </c>
       <c r="L7" s="146">
-        <f>K7*46</f>
+        <f t="shared" si="0"/>
         <v>3496</v>
       </c>
       <c r="M7" s="142"/>
@@ -13213,7 +13213,7 @@
         <v>51</v>
       </c>
       <c r="L8" s="146">
-        <f>K8*46</f>
+        <f t="shared" si="0"/>
         <v>2346</v>
       </c>
       <c r="M8" s="142"/>
@@ -13255,7 +13255,7 @@
         <v>34.6</v>
       </c>
       <c r="L9" s="146">
-        <f>K9*46</f>
+        <f t="shared" si="0"/>
         <v>1591.6000000000001</v>
       </c>
       <c r="M9" s="142"/>
@@ -13297,7 +13297,7 @@
         <v>49.6</v>
       </c>
       <c r="L10" s="146">
-        <f>K10*46</f>
+        <f t="shared" si="0"/>
         <v>2281.6</v>
       </c>
       <c r="M10" s="142"/>
@@ -13339,7 +13339,7 @@
         <v>57</v>
       </c>
       <c r="L11" s="146">
-        <f>K11*46</f>
+        <f t="shared" si="0"/>
         <v>2622</v>
       </c>
       <c r="M11" s="142"/>
@@ -13381,7 +13381,7 @@
         <v>18.3</v>
       </c>
       <c r="L12" s="146">
-        <f>K12*46</f>
+        <f t="shared" si="0"/>
         <v>841.80000000000007</v>
       </c>
       <c r="M12" s="142"/>
@@ -13423,7 +13423,7 @@
         <v>19.600000000000001</v>
       </c>
       <c r="L13" s="146">
-        <f>K13*46</f>
+        <f t="shared" si="0"/>
         <v>901.6</v>
       </c>
       <c r="M13" s="142"/>

</xml_diff>